<commit_message>
Manual Renter All Stocks
</commit_message>
<xml_diff>
--- a/login.xlsx
+++ b/login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murar\Downloads\Freelancing\Short-Straddle-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CCD73D-63DE-4E14-8E12-0D63A4B734F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6C5256-EAE4-45E4-B843-C290E30C3B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>short straddle</t>
+  </si>
+  <si>
+    <t>long straddle</t>
+  </si>
+  <si>
+    <t>Long Straddle Status</t>
   </si>
 </sst>
 </file>
@@ -408,19 +414,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
     <col min="4" max="4" width="43.88671875" customWidth="1"/>
+    <col min="5" max="5" width="31.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +443,14 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>